<commit_message>
dev-197 - fixed parse dttm
</commit_message>
<xml_diff>
--- a/etc/scripts/demand.xlsx
+++ b/etc/scripts/demand.xlsx
@@ -1,31 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38397343-38F6-404D-94C5-A99EA999D8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="480" windowWidth="25260" windowHeight="13540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="2019.05.30-2019.06.02" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -38,13 +22,16 @@
     <t>Время</t>
   </si>
   <si>
+    <t>Значение</t>
+  </si>
+  <si>
+    <t>* первая строка содержит название столбцов</t>
+  </si>
+  <si>
     <t>Кассы</t>
   </si>
   <si>
-    <t>Значение</t>
-  </si>
-  <si>
-    <t>Торговый зал</t>
+    <t>* В данном случае пример магазина, который работает с 10 до 21, где есть 2 типа работ: кассы и торговый зал. И заносим необходимое количество сотрудников по 2 типам работ на 30 арпеля-1мая.</t>
   </si>
   <si>
     <t>* первый столбец содержит тип работ, второй -- время ,третий --  количество сотрудников, которое нужно в это время на этот вид работ</t>
@@ -53,40 +40,381 @@
     <t>* порядок строк не имеет значения</t>
   </si>
   <si>
+    <t>* для составления графика выхода сотрудников необходимо указывать информацию на целый месяц</t>
+  </si>
+  <si>
     <t>* для корректировки нагрузки в какой-то период, достаточно загрузить данные за этот период</t>
   </si>
   <si>
-    <t>* первая строка содержит название столбцов</t>
-  </si>
-  <si>
-    <t>* для составления графика выхода сотрудников необходимо указывать информацию на целый месяц</t>
-  </si>
-  <si>
-    <t>* В данном случае пример магазина, который работает с 10 до 21, где есть 2 типа работ: кассы и торговый зал. И заносим необходимое количество сотрудников по 2 типам работ на 30 арпеля-1мая.</t>
+    <t>Торговый зал</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -94,25 +422,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -161,7 +775,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,26 +808,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,23 +843,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -433,25 +1013,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="1" max="3" width="30.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="18.1666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,29 +1039,29 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>43951.416666666664</v>
+        <v>43951.4166666667</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>43951.5</v>
@@ -490,40 +1070,40 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>43951.541666666664</v>
+        <v>43951.5416666667</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>43951.583333333336</v>
+        <v>43951.5833333333</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>43951.625</v>
@@ -532,34 +1112,34 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>43951.666666666664</v>
+        <v>43951.6666666667</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>43951.708333333336</v>
+        <v>43951.7083333333</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>43951.75</v>
@@ -568,43 +1148,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>43951.791666666664</v>
+        <v>43951.7916666667</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>43951.833333333336</v>
+        <v>43951.8333333333</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1">
         <f>B2+1</f>
-        <v>43952.416666666664</v>
+        <v>43952.4166666667</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" ref="B13:B21" si="0">B3+1</f>
@@ -614,33 +1194,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>43952.541666666664</v>
+        <v>43952.5416666667</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>43952.583333333336</v>
+        <v>43952.5833333333</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
@@ -650,33 +1230,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>43952.666666666664</v>
+        <v>43952.6666666667</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>43952.708333333336</v>
+        <v>43952.7083333333</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
@@ -686,44 +1266,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>43952.791666666664</v>
+        <v>43952.7916666667</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>43952.833333333336</v>
+        <v>43952.8333333333</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
-        <v>43951.416666666664</v>
+        <v>43951.4166666667</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1">
         <v>43951.5</v>
@@ -732,31 +1312,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1">
-        <v>43951.541666666664</v>
+        <v>43951.5416666667</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B25" s="1">
-        <v>43951.583333333336</v>
+        <v>43951.5833333333</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1">
         <v>43951.625</v>
@@ -765,31 +1345,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1">
-        <v>43951.666666666664</v>
+        <v>43951.6666666667</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1">
-        <v>43951.708333333336</v>
+        <v>43951.7083333333</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B29" s="1">
         <v>43951.75</v>
@@ -798,43 +1378,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1">
-        <v>43951.791666666664</v>
+        <v>43951.7916666667</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1">
-        <v>43951.833333333336</v>
+        <v>43951.8333333333</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1">
         <f>B22+1</f>
-        <v>43952.416666666664</v>
+        <v>43952.4166666667</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <f t="shared" ref="B33:B41" si="1">B23+1</f>
@@ -844,33 +1424,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1">
         <f t="shared" si="1"/>
-        <v>43952.541666666664</v>
+        <v>43952.5416666667</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1">
         <f t="shared" si="1"/>
-        <v>43952.583333333336</v>
+        <v>43952.5833333333</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B36" s="1">
         <f t="shared" si="1"/>
@@ -880,33 +1460,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1">
         <f t="shared" si="1"/>
-        <v>43952.666666666664</v>
+        <v>43952.6666666667</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B38" s="1">
         <f t="shared" si="1"/>
-        <v>43952.708333333336</v>
+        <v>43952.7083333333</v>
       </c>
       <c r="C38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B39" s="1">
         <f t="shared" si="1"/>
@@ -916,25 +1496,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B40" s="1">
         <f t="shared" si="1"/>
-        <v>43952.791666666664</v>
+        <v>43952.7916666667</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1">
         <f t="shared" si="1"/>
-        <v>43952.833333333336</v>
+        <v>43952.8333333333</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -942,5 +1522,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>